<commit_message>
remove unused file combine configure file of server
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Language.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Language.xlsx
@@ -5,14 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Ini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Comm" sheetId="1" r:id="rId1"/>
+    <sheet name="Property" sheetId="7" r:id="rId2"/>
+    <sheet name="Guild" sheetId="3" r:id="rId3"/>
+    <sheet name="Tip" sheetId="4" r:id="rId4"/>
+    <sheet name="Item" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -83,23 +87,79 @@
     <t>Langage_6</t>
   </si>
   <si>
-    <t>中文_1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>中文_2</t>
-  </si>
-  <si>
-    <t>中文_3</t>
-  </si>
-  <si>
-    <t>中文_4</t>
-  </si>
-  <si>
-    <t>中文_5</t>
+    <t>Langage_Guild_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>确认要加入这个公会吗？点击确认加入</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>确认</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建角色</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入游戏</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Langage_Comm_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Langage_Comm_2</t>
+  </si>
+  <si>
+    <t>Langage_Comm_3</t>
+  </si>
+  <si>
+    <t>Langage_Comm_4</t>
+  </si>
+  <si>
+    <t>Langage_Comm_5</t>
+  </si>
+  <si>
+    <t>Langage_Comm_6</t>
   </si>
   <si>
     <t>中文_6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Langage_HP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Langage_MP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Langage_VP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Langage_MAXHP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Langage_MAXMP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Langage_ATTACK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -505,17 +565,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:I1048576"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.125" customWidth="1"/>
-    <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.875" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
@@ -531,69 +591,94 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -601,4 +686,283 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="51.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="31.875" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>